<commit_message>
Pin LUT updated and bugs noted.
</commit_message>
<xml_diff>
--- a/circuit_diagrams/easyEDA/pin_LUT.xlsx
+++ b/circuit_diagrams/easyEDA/pin_LUT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dougal/src/TBAG/circuit_diagrams/easyEDA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F8B64B1-FDC6-134B-903B-F020A00F68C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A56E1050-B22D-8742-96D5-4E34F16FDB1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="18840" windowHeight="17800" xr2:uid="{2DC34212-85A1-C04D-97E8-8B951958887B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>Desc</t>
   </si>
@@ -53,16 +53,157 @@
   </si>
   <si>
     <t>Eng 2 LP 3</t>
+  </si>
+  <si>
+    <t>Eng 1 LP 2</t>
+  </si>
+  <si>
+    <t>Eng 1 LP 3</t>
+  </si>
+  <si>
+    <t>Eng 2 LP 1</t>
+  </si>
+  <si>
+    <t>Eng 2 LP 2</t>
+  </si>
+  <si>
+    <t>Eng 2 HP 1</t>
+  </si>
+  <si>
+    <t>Eng 2 HP 2</t>
+  </si>
+  <si>
+    <t>Eng 2 HP 3</t>
+  </si>
+  <si>
+    <t>Eng 1 HP 1</t>
+  </si>
+  <si>
+    <t>Eng 1 HP 2</t>
+  </si>
+  <si>
+    <t>Eng 1 HP 3</t>
+  </si>
+  <si>
+    <t>Eng 1 TGT -</t>
+  </si>
+  <si>
+    <t>Eng 1 TGT +</t>
+  </si>
+  <si>
+    <t>Eng 2 TGT -</t>
+  </si>
+  <si>
+    <t>Eng 2 TGT +</t>
+  </si>
+  <si>
+    <t>Eng 1 Throt +</t>
+  </si>
+  <si>
+    <t>Eng 1 Throt -</t>
+  </si>
+  <si>
+    <t>Eng 1 Throt out</t>
+  </si>
+  <si>
+    <t>Eng 2 Throt -</t>
+  </si>
+  <si>
+    <t>Eng 2 Throt +</t>
+  </si>
+  <si>
+    <t>Eng 2 Throt out</t>
+  </si>
+  <si>
+    <t>Air start</t>
+  </si>
+  <si>
+    <t>Eng 1 Master</t>
+  </si>
+  <si>
+    <t>Eng 2 Master</t>
+  </si>
+  <si>
+    <t>Eng 1 Fuel cock</t>
+  </si>
+  <si>
+    <t>Eng 2 fuel cock</t>
+  </si>
+  <si>
+    <t>5V, air start</t>
+  </si>
+  <si>
+    <t>5V, Eng 2 fuel cock</t>
+  </si>
+  <si>
+    <t>5V, Eng 1 Fuel cock</t>
+  </si>
+  <si>
+    <t>5V, Eng 1 Master</t>
+  </si>
+  <si>
+    <t>5V, Eng 2 Master</t>
+  </si>
+  <si>
+    <t>Eng 2 oil press 1</t>
+  </si>
+  <si>
+    <t>Eng 2 oil press 2</t>
+  </si>
+  <si>
+    <t>Eng 2 oil press 3</t>
+  </si>
+  <si>
+    <t>Eng 1 oil press 1</t>
+  </si>
+  <si>
+    <t>Eng 1 oil press 2</t>
+  </si>
+  <si>
+    <t>Eng 1 oil press 3</t>
+  </si>
+  <si>
+    <t>LP spin +</t>
+  </si>
+  <si>
+    <t>LP spin - (gap)</t>
+  </si>
+  <si>
+    <t>Eng 1 start</t>
+  </si>
+  <si>
+    <t>Eng 2 start</t>
+  </si>
+  <si>
+    <t>5V, Eng 2 start</t>
+  </si>
+  <si>
+    <t>5V, Eng 1 start</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -88,8 +229,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,26 +549,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C5F6AB7-B68F-304A-A806-E2AAE5ADA0C8}">
   <dimension ref="A3:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32:B47"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -458,6 +604,9 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
       <c r="B6">
         <v>8</v>
       </c>
@@ -466,6 +615,9 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B7">
         <v>8</v>
       </c>
@@ -474,6 +626,9 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B8">
         <v>8</v>
       </c>
@@ -482,6 +637,9 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B9">
         <v>8</v>
       </c>
@@ -490,6 +648,9 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B10">
         <v>8</v>
       </c>
@@ -498,6 +659,9 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B11">
         <v>8</v>
       </c>
@@ -506,6 +670,9 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B12">
         <v>8</v>
       </c>
@@ -514,6 +681,9 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="B13">
         <v>8</v>
       </c>
@@ -522,6 +692,9 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B14">
         <v>8</v>
       </c>
@@ -530,6 +703,9 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="B15">
         <v>8</v>
       </c>
@@ -538,6 +714,9 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B16">
         <v>8</v>
       </c>
@@ -545,7 +724,10 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="B17">
         <v>8</v>
       </c>
@@ -553,7 +735,10 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
       <c r="B18">
         <v>8</v>
       </c>
@@ -561,7 +746,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="B19">
         <v>8</v>
       </c>
@@ -569,7 +757,10 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="B20">
         <v>10</v>
       </c>
@@ -577,7 +768,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="B21">
         <v>10</v>
       </c>
@@ -585,7 +779,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="B22">
         <v>10</v>
       </c>
@@ -593,7 +790,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="B23">
         <v>10</v>
       </c>
@@ -601,7 +801,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="B24">
         <v>10</v>
       </c>
@@ -609,7 +812,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="B25">
         <v>10</v>
       </c>
@@ -617,7 +823,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="B26">
         <v>10</v>
       </c>
@@ -625,7 +834,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="B27">
         <v>10</v>
       </c>
@@ -633,7 +845,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="B28">
         <v>10</v>
       </c>
@@ -641,7 +856,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="B29">
         <v>10</v>
       </c>
@@ -649,7 +867,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="B30">
         <v>10</v>
       </c>
@@ -657,7 +878,10 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="B31">
         <v>10</v>
       </c>
@@ -665,7 +889,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>20</v>
+      </c>
       <c r="B32">
         <v>9</v>
       </c>
@@ -673,7 +900,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>27</v>
+      </c>
       <c r="B33">
         <v>9</v>
       </c>
@@ -681,7 +911,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>21</v>
+      </c>
       <c r="B34">
         <v>9</v>
       </c>
@@ -689,7 +922,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
       <c r="B35">
         <v>9</v>
       </c>
@@ -697,7 +933,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>22</v>
+      </c>
       <c r="B36">
         <v>9</v>
       </c>
@@ -705,7 +944,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>28</v>
+      </c>
       <c r="B37">
         <v>9</v>
       </c>
@@ -713,7 +955,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>24</v>
+      </c>
       <c r="B38">
         <v>9</v>
       </c>
@@ -721,7 +966,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="B39">
         <v>9</v>
       </c>
@@ -729,7 +977,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>23</v>
+      </c>
       <c r="B40">
         <v>9</v>
       </c>
@@ -737,7 +988,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>29</v>
+      </c>
       <c r="B41">
         <v>9</v>
       </c>
@@ -745,7 +999,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>25</v>
+      </c>
       <c r="B42">
         <v>9</v>
       </c>
@@ -753,7 +1010,10 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>33</v>
+      </c>
       <c r="B43">
         <v>9</v>
       </c>
@@ -761,7 +1021,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>32</v>
+      </c>
       <c r="B44">
         <v>9</v>
       </c>
@@ -769,7 +1032,10 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>30</v>
+      </c>
       <c r="B45">
         <v>9</v>
       </c>
@@ -777,7 +1043,10 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>26</v>
+      </c>
       <c r="B46">
         <v>9</v>
       </c>
@@ -785,7 +1054,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>31</v>
+      </c>
       <c r="B47">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Pins updated after soldering.
</commit_message>
<xml_diff>
--- a/circuit_diagrams/easyEDA/pin_LUT.xlsx
+++ b/circuit_diagrams/easyEDA/pin_LUT.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dougal/src/TBAG/circuit_diagrams/easyEDA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12272A65-2A42-3040-9917-244E88D171A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB82CAD9-284D-3043-A478-7352763F7D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="18840" windowHeight="17800" xr2:uid="{2DC34212-85A1-C04D-97E8-8B951958887B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="48">
   <si>
     <t>Desc</t>
   </si>
@@ -547,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C5F6AB7-B68F-304A-A806-E2AAE5ADA0C8}">
-  <dimension ref="A3:E47"/>
+  <dimension ref="A3:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="J48" sqref="J48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -558,7 +558,7 @@
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -574,8 +574,24 @@
       <c r="E3" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" s="2"/>
+      <c r="H3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -589,10 +605,25 @@
         <v>1</v>
       </c>
       <c r="E4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="H4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4">
+        <v>8</v>
+      </c>
+      <c r="J4">
+        <v>10</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -606,10 +637,25 @@
         <v>1</v>
       </c>
       <c r="E5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="H5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5">
+        <v>8</v>
+      </c>
+      <c r="J5">
+        <v>8</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -623,10 +669,25 @@
         <v>1</v>
       </c>
       <c r="E6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="H6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6">
+        <v>8</v>
+      </c>
+      <c r="J6">
+        <v>6</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -640,10 +701,25 @@
         <v>1</v>
       </c>
       <c r="E7">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="H7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7">
+        <v>8</v>
+      </c>
+      <c r="J7">
+        <v>4</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -657,10 +733,25 @@
         <v>1</v>
       </c>
       <c r="E8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="H8" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8">
+        <v>8</v>
+      </c>
+      <c r="J8">
+        <v>2</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -674,10 +765,25 @@
         <v>1</v>
       </c>
       <c r="E9">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="H9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9">
+        <v>8</v>
+      </c>
+      <c r="J9">
+        <v>15</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -691,10 +797,25 @@
         <v>1</v>
       </c>
       <c r="E10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="H10" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10">
+        <v>8</v>
+      </c>
+      <c r="J10">
+        <v>13</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -708,10 +829,25 @@
         <v>1</v>
       </c>
       <c r="E11">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="H11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11">
+        <v>8</v>
+      </c>
+      <c r="J11">
+        <v>11</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -725,10 +861,25 @@
         <v>1</v>
       </c>
       <c r="E12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="H12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12">
+        <v>8</v>
+      </c>
+      <c r="J12">
+        <v>9</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
@@ -742,10 +893,25 @@
         <v>1</v>
       </c>
       <c r="E13">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="H13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13">
+        <v>8</v>
+      </c>
+      <c r="J13">
+        <v>7</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -759,10 +925,25 @@
         <v>1</v>
       </c>
       <c r="E14">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="H14" t="s">
+        <v>7</v>
+      </c>
+      <c r="I14">
+        <v>8</v>
+      </c>
+      <c r="J14">
+        <v>5</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -776,10 +957,25 @@
         <v>1</v>
       </c>
       <c r="E15">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="H15" t="s">
+        <v>6</v>
+      </c>
+      <c r="I15">
+        <v>8</v>
+      </c>
+      <c r="J15">
+        <v>3</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
@@ -795,8 +991,23 @@
       <c r="E16">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H16" t="s">
+        <v>4</v>
+      </c>
+      <c r="I16">
+        <v>8</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -810,10 +1021,25 @@
         <v>1</v>
       </c>
       <c r="E17">
+        <v>15</v>
+      </c>
+      <c r="H17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="I17">
+        <v>8</v>
+      </c>
+      <c r="J17">
+        <v>12</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -827,10 +1053,25 @@
         <v>1</v>
       </c>
       <c r="E18">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="H18" t="s">
+        <v>19</v>
+      </c>
+      <c r="I18">
+        <v>8</v>
+      </c>
+      <c r="J18">
+        <v>14</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -844,10 +1085,25 @@
         <v>1</v>
       </c>
       <c r="E19">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="H19" t="s">
+        <v>18</v>
+      </c>
+      <c r="I19">
+        <v>8</v>
+      </c>
+      <c r="J19">
+        <v>16</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>39</v>
       </c>
@@ -863,8 +1119,23 @@
       <c r="E20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H20" t="s">
+        <v>20</v>
+      </c>
+      <c r="I20">
+        <v>9</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>42</v>
       </c>
@@ -880,8 +1151,23 @@
       <c r="E21">
         <v>7</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H21" t="s">
+        <v>21</v>
+      </c>
+      <c r="I21">
+        <v>9</v>
+      </c>
+      <c r="J21">
+        <v>3</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>40</v>
       </c>
@@ -897,8 +1183,23 @@
       <c r="E22">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H22" t="s">
+        <v>22</v>
+      </c>
+      <c r="I22">
+        <v>9</v>
+      </c>
+      <c r="J22">
+        <v>5</v>
+      </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="L22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>43</v>
       </c>
@@ -914,8 +1215,23 @@
       <c r="E23">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H23" t="s">
+        <v>24</v>
+      </c>
+      <c r="I23">
+        <v>9</v>
+      </c>
+      <c r="J23">
+        <v>7</v>
+      </c>
+      <c r="K23">
+        <v>1</v>
+      </c>
+      <c r="L23">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>41</v>
       </c>
@@ -931,8 +1247,23 @@
       <c r="E24">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H24" t="s">
+        <v>23</v>
+      </c>
+      <c r="I24">
+        <v>9</v>
+      </c>
+      <c r="J24">
+        <v>9</v>
+      </c>
+      <c r="K24">
+        <v>1</v>
+      </c>
+      <c r="L24">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>44</v>
       </c>
@@ -948,8 +1279,23 @@
       <c r="E25">
         <v>9</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H25" t="s">
+        <v>25</v>
+      </c>
+      <c r="I25">
+        <v>9</v>
+      </c>
+      <c r="J25">
+        <v>11</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="L25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>36</v>
       </c>
@@ -965,8 +1311,23 @@
       <c r="E26">
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H26" t="s">
+        <v>26</v>
+      </c>
+      <c r="I26">
+        <v>9</v>
+      </c>
+      <c r="J26">
+        <v>15</v>
+      </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="L26">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>47</v>
       </c>
@@ -982,8 +1343,23 @@
       <c r="E27">
         <v>10</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H27" t="s">
+        <v>31</v>
+      </c>
+      <c r="I27">
+        <v>9</v>
+      </c>
+      <c r="J27">
+        <v>16</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>37</v>
       </c>
@@ -999,8 +1375,23 @@
       <c r="E28">
         <v>5</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H28" t="s">
+        <v>39</v>
+      </c>
+      <c r="I28">
+        <v>10</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28">
+        <v>2</v>
+      </c>
+      <c r="L28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>45</v>
       </c>
@@ -1016,8 +1407,23 @@
       <c r="E29">
         <v>11</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H29" t="s">
+        <v>40</v>
+      </c>
+      <c r="I29">
+        <v>10</v>
+      </c>
+      <c r="J29">
+        <v>3</v>
+      </c>
+      <c r="K29">
+        <v>2</v>
+      </c>
+      <c r="L29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>38</v>
       </c>
@@ -1033,8 +1439,23 @@
       <c r="E30">
         <v>6</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H30" t="s">
+        <v>41</v>
+      </c>
+      <c r="I30">
+        <v>10</v>
+      </c>
+      <c r="J30">
+        <v>5</v>
+      </c>
+      <c r="K30">
+        <v>2</v>
+      </c>
+      <c r="L30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>46</v>
       </c>
@@ -1050,8 +1471,23 @@
       <c r="E31">
         <v>12</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H31" t="s">
+        <v>36</v>
+      </c>
+      <c r="I31">
+        <v>10</v>
+      </c>
+      <c r="J31">
+        <v>7</v>
+      </c>
+      <c r="K31">
+        <v>2</v>
+      </c>
+      <c r="L31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>20</v>
       </c>
@@ -1067,8 +1503,23 @@
       <c r="E32">
         <v>18</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H32" t="s">
+        <v>37</v>
+      </c>
+      <c r="I32">
+        <v>10</v>
+      </c>
+      <c r="J32">
+        <v>9</v>
+      </c>
+      <c r="K32">
+        <v>2</v>
+      </c>
+      <c r="L32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>27</v>
       </c>
@@ -1084,8 +1535,23 @@
       <c r="E33">
         <v>13</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H33" t="s">
+        <v>38</v>
+      </c>
+      <c r="I33">
+        <v>10</v>
+      </c>
+      <c r="J33">
+        <v>11</v>
+      </c>
+      <c r="K33">
+        <v>2</v>
+      </c>
+      <c r="L33">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>21</v>
       </c>
@@ -1101,8 +1567,23 @@
       <c r="E34">
         <v>19</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H34" t="s">
+        <v>42</v>
+      </c>
+      <c r="I34">
+        <v>10</v>
+      </c>
+      <c r="J34">
+        <v>2</v>
+      </c>
+      <c r="K34">
+        <v>2</v>
+      </c>
+      <c r="L34">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1118,8 +1599,23 @@
       <c r="E35">
         <v>14</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H35" t="s">
+        <v>43</v>
+      </c>
+      <c r="I35">
+        <v>10</v>
+      </c>
+      <c r="J35">
+        <v>4</v>
+      </c>
+      <c r="K35">
+        <v>2</v>
+      </c>
+      <c r="L35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -1135,8 +1631,23 @@
       <c r="E36">
         <v>20</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H36" t="s">
+        <v>44</v>
+      </c>
+      <c r="I36">
+        <v>10</v>
+      </c>
+      <c r="J36">
+        <v>6</v>
+      </c>
+      <c r="K36">
+        <v>2</v>
+      </c>
+      <c r="L36">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>28</v>
       </c>
@@ -1152,8 +1663,23 @@
       <c r="E37">
         <v>15</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H37" t="s">
+        <v>47</v>
+      </c>
+      <c r="I37">
+        <v>10</v>
+      </c>
+      <c r="J37">
+        <v>8</v>
+      </c>
+      <c r="K37">
+        <v>2</v>
+      </c>
+      <c r="L37">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -1169,8 +1695,23 @@
       <c r="E38">
         <v>21</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H38" t="s">
+        <v>45</v>
+      </c>
+      <c r="I38">
+        <v>9</v>
+      </c>
+      <c r="J38">
+        <v>6</v>
+      </c>
+      <c r="K38">
+        <v>2</v>
+      </c>
+      <c r="L38">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>35</v>
       </c>
@@ -1186,8 +1727,23 @@
       <c r="E39">
         <v>16</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H39" t="s">
+        <v>46</v>
+      </c>
+      <c r="I39">
+        <v>9</v>
+      </c>
+      <c r="J39">
+        <v>4</v>
+      </c>
+      <c r="K39">
+        <v>2</v>
+      </c>
+      <c r="L39">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>23</v>
       </c>
@@ -1203,8 +1759,23 @@
       <c r="E40">
         <v>22</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H40" t="s">
+        <v>27</v>
+      </c>
+      <c r="I40">
+        <v>9</v>
+      </c>
+      <c r="J40">
+        <v>2</v>
+      </c>
+      <c r="K40">
+        <v>2</v>
+      </c>
+      <c r="L40">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>29</v>
       </c>
@@ -1220,8 +1791,23 @@
       <c r="E41">
         <v>17</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H41" t="s">
+        <v>34</v>
+      </c>
+      <c r="I41">
+        <v>9</v>
+      </c>
+      <c r="J41">
+        <v>8</v>
+      </c>
+      <c r="K41">
+        <v>2</v>
+      </c>
+      <c r="L41">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>25</v>
       </c>
@@ -1237,8 +1823,23 @@
       <c r="E42">
         <v>23</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H42" t="s">
+        <v>28</v>
+      </c>
+      <c r="I42">
+        <v>9</v>
+      </c>
+      <c r="J42">
+        <v>10</v>
+      </c>
+      <c r="K42">
+        <v>2</v>
+      </c>
+      <c r="L42">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>33</v>
       </c>
@@ -1254,8 +1855,23 @@
       <c r="E43">
         <v>18</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H43" t="s">
+        <v>35</v>
+      </c>
+      <c r="I43">
+        <v>9</v>
+      </c>
+      <c r="J43">
+        <v>12</v>
+      </c>
+      <c r="K43">
+        <v>2</v>
+      </c>
+      <c r="L43">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>32</v>
       </c>
@@ -1271,8 +1887,23 @@
       <c r="E44">
         <v>20</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H44" t="s">
+        <v>29</v>
+      </c>
+      <c r="I44">
+        <v>9</v>
+      </c>
+      <c r="J44">
+        <v>14</v>
+      </c>
+      <c r="K44">
+        <v>2</v>
+      </c>
+      <c r="L44">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>30</v>
       </c>
@@ -1288,8 +1919,23 @@
       <c r="E45">
         <v>19</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H45" t="s">
+        <v>33</v>
+      </c>
+      <c r="I45">
+        <v>9</v>
+      </c>
+      <c r="J45">
+        <v>13</v>
+      </c>
+      <c r="K45">
+        <v>2</v>
+      </c>
+      <c r="L45">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>26</v>
       </c>
@@ -1305,8 +1951,23 @@
       <c r="E46">
         <v>24</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H46" t="s">
+        <v>30</v>
+      </c>
+      <c r="I46">
+        <v>10</v>
+      </c>
+      <c r="J46">
+        <v>10</v>
+      </c>
+      <c r="K46">
+        <v>2</v>
+      </c>
+      <c r="L46">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>31</v>
       </c>
@@ -1322,8 +1983,26 @@
       <c r="E47">
         <v>25</v>
       </c>
+      <c r="H47" t="s">
+        <v>32</v>
+      </c>
+      <c r="I47">
+        <v>9</v>
+      </c>
+      <c r="J47">
+        <v>12</v>
+      </c>
+      <c r="K47">
+        <v>2</v>
+      </c>
+      <c r="L47">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H29:L47">
+    <sortCondition ref="L29:L47"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Notes added to pin LUT.
</commit_message>
<xml_diff>
--- a/circuit_diagrams/easyEDA/pin_LUT.xlsx
+++ b/circuit_diagrams/easyEDA/pin_LUT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dougal/src/TBAG/circuit_diagrams/easyEDA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB82CAD9-284D-3043-A478-7352763F7D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0918EB1-3333-8745-A94C-A9F1CC28E16F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="18840" windowHeight="17800" xr2:uid="{2DC34212-85A1-C04D-97E8-8B951958887B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="51">
   <si>
     <t>Desc</t>
   </si>
@@ -179,6 +179,15 @@
   </si>
   <si>
     <t>5V, Eng 1 start</t>
+  </si>
+  <si>
+    <t>I think it is this one. Check</t>
+  </si>
+  <si>
+    <t>Arduino pin</t>
+  </si>
+  <si>
+    <t>Arduino in/out</t>
   </si>
 </sst>
 </file>
@@ -547,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C5F6AB7-B68F-304A-A806-E2AAE5ADA0C8}">
-  <dimension ref="A3:L47"/>
+  <dimension ref="A2:N47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="J48" sqref="J48"/>
+    <sheetView tabSelected="1" topLeftCell="B32" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -558,7 +567,16 @@
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -575,23 +593,29 @@
         <v>2</v>
       </c>
       <c r="F3" s="2"/>
-      <c r="H3" t="s">
+      <c r="H3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I3" t="s">
-        <v>1</v>
-      </c>
-      <c r="J3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="I3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="L3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -623,7 +647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -655,7 +679,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -687,7 +711,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -719,7 +743,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -751,7 +775,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -783,7 +807,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -815,7 +839,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -847,7 +871,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -879,7 +903,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
@@ -911,7 +935,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -943,7 +967,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -975,7 +999,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>

</xml_diff>